<commit_message>
Proyecto de procesamiento de datos Jesus_f
</commit_message>
<xml_diff>
--- a/Parametros.xlsx
+++ b/Parametros.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\home\OneDrive\Escritorio\Esp. IA\Deep Learning\entregable\Proyecto1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Especializacion\Procesamieto de Datos Secuenciales\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t>LSTM</t>
   </si>
@@ -358,6 +358,12 @@
   </si>
   <si>
     <t>Parametros=2×embedding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lstm (LSTM) </t>
+  </si>
+  <si>
+    <t>Paraˊmetros=4×(Dimensioˊn del embedding+Unidades GRU)×Unidades GRU    +  Sesgos</t>
   </si>
 </sst>
 </file>
@@ -718,15 +724,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1009,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1051,10 +1057,10 @@
     </row>
     <row r="4" spans="1:4" ht="28.8">
       <c r="A4" s="19" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C4" s="6"/>
     </row>
@@ -1190,11 +1196,11 @@
       <c r="C20" s="12"/>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
@@ -1334,11 +1340,11 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
@@ -1384,20 +1390,20 @@
       <c r="A43" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="29" t="s">
         <v>40</v>
       </c>
       <c r="C43" s="25"/>
     </row>
     <row r="44" spans="1:4" ht="15.6">
       <c r="A44" s="19"/>
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C44" s="25">
         <v>263808</v>
       </c>
-      <c r="D44" s="28"/>
+      <c r="D44" s="27"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="19" t="s">
@@ -1450,7 +1456,7 @@
     </row>
     <row r="50" spans="1:3" ht="15">
       <c r="A50" s="19"/>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="30" t="s">
         <v>42</v>
       </c>
       <c r="C50" s="25">

</xml_diff>